<commit_message>
Nop Commerce project Prio 1
</commit_message>
<xml_diff>
--- a/NopCommerce/Test_Suites/TC_LoginTest_Report.xlsx
+++ b/NopCommerce/Test_Suites/TC_LoginTest_Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>Valid Email &amp; Password</t>
-  </si>
-  <si>
-    <t>ahmed.magdy.dawam@gmail.com</t>
-  </si>
-  <si>
-    <t>5UL4EwiHWHh@EN</t>
   </si>
   <si>
     <t>Navigate to Home page</t>
@@ -514,7 +508,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -563,13 +557,13 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -577,19 +571,19 @@
     </row>
     <row r="3" spans="1:8" ht="33.75" customHeight="1" thickBot="1">
       <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -597,19 +591,19 @@
     </row>
     <row r="4" spans="1:8" ht="33.75" customHeight="1" thickBot="1">
       <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -625,8 +619,9 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>